<commit_message>
Se actualiza diccionario de datos
</commit_message>
<xml_diff>
--- a/diccionario_datos/diccionario_datos_sniim.xlsx
+++ b/diccionario_datos/diccionario_datos_sniim.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janneth\Documents\MCD\Semestre1\Ing. de Características\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Janneth\Documents\MCD\Semestre1\Ing. de Características\RedBAMX\diccionario_datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7AB395-34AA-4C2B-98DB-369AA9C0C404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48F227F-3047-44C2-B5E3-DD659D920297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2005" yWindow="985" windowWidth="14635" windowHeight="10000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejemplo_diccionario de datos" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="58">
   <si>
     <r>
       <rPr>
@@ -313,36 +313,12 @@
     <t>SNIIM</t>
   </si>
   <si>
-    <t>Presentación</t>
-  </si>
-  <si>
-    <t>Origen</t>
-  </si>
-  <si>
-    <t>Destino</t>
-  </si>
-  <si>
-    <t>PrecioMin</t>
-  </si>
-  <si>
-    <t>PrecioMax</t>
-  </si>
-  <si>
-    <t>PrecioFrec</t>
-  </si>
-  <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
     <t>dd/mm/aaaa</t>
   </si>
   <si>
     <t>Lugar de donde proviene el producto. En este caso se refiere a la entidad federativa.</t>
   </si>
   <si>
-    <t>Lugar donde se captura el precio del producto. En este caso se indica el nombre de la entidad federativa y el nombre del centro mayorista o central de abasto.</t>
-  </si>
-  <si>
     <t>Fecha en que se captura el precio del producto.</t>
   </si>
   <si>
@@ -370,13 +346,46 @@
     <t>df_sniim_fyh</t>
   </si>
   <si>
-    <t>Producto</t>
-  </si>
-  <si>
     <t>El nombre del producto.</t>
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>fecha</t>
+  </si>
+  <si>
+    <t>presentación</t>
+  </si>
+  <si>
+    <t>origen</t>
+  </si>
+  <si>
+    <t>precio_min</t>
+  </si>
+  <si>
+    <t>precio_max</t>
+  </si>
+  <si>
+    <t>precio_frec</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>estado_destino</t>
+  </si>
+  <si>
+    <t>lugar_destino</t>
+  </si>
+  <si>
+    <t>Entidad federativa donde se captura el precio del producto.</t>
+  </si>
+  <si>
+    <t>Nombre del centro mayorista o central de abasto donde se captura el precio del producto.</t>
   </si>
 </sst>
 </file>
@@ -595,7 +604,7 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -826,11 +835,11 @@
     <tabColor rgb="FF57BB8A"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.20703125" defaultRowHeight="15" customHeight="1"/>
@@ -880,25 +889,25 @@
         <v>32</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>12</v>
@@ -912,13 +921,13 @@
         <v>32</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>14</v>
@@ -930,7 +939,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>12</v>
@@ -944,13 +953,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>14</v>
@@ -962,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>12</v>
@@ -971,30 +980,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="71.75">
+    <row r="5" spans="1:11" ht="36.5">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>12</v>
@@ -1008,25 +1017,25 @@
         <v>32</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>12</v>
@@ -1035,30 +1044,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="36.5">
+    <row r="7" spans="1:11" ht="24.75">
       <c r="A7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>12</v>
@@ -1067,50 +1076,51 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="24.75">
+    <row r="8" spans="1:11" ht="16">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="16">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>14</v>
@@ -1122,28 +1132,27 @@
         <v>11</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="16">
+        <v>12</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="24.75">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>14</v>
@@ -1155,7 +1164,7 @@
         <v>11</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>12</v>
@@ -1164,8 +1173,40 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11" spans="1:11" ht="36.5">
+      <c r="A11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E10">
+  <conditionalFormatting sqref="E2:E11">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(E2))&gt;0</formula>
     </cfRule>
@@ -1178,19 +1219,19 @@
           <x14:formula1>
             <xm:f>Validadores!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G10</xm:sqref>
+          <xm:sqref>G2:G11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>Validadores!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E10</xm:sqref>
+          <xm:sqref>E2:E11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Validadores!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I10</xm:sqref>
+          <xm:sqref>I2:I11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>